<commit_message>
Update Excel parameters 2
</commit_message>
<xml_diff>
--- a/input_parameter.xlsx
+++ b/input_parameter.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b605f118ad36e084/FHNW/intern_SimProg/test_simprog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="325" documentId="13_ncr:1_{6DA2A0BF-A077-4220-9EAC-603438CCD898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B19F3C8A-7AD6-4DE8-A465-83C248B69F6D}"/>
+  <xr:revisionPtr revIDLastSave="331" documentId="13_ncr:1_{6DA2A0BF-A077-4220-9EAC-603438CCD898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9382707A-116C-4EC5-B1E4-1E89A285EB6D}"/>
   <bookViews>
-    <workbookView xWindow="-16425" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16425" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="201">
   <si>
     <t>Beschreibung</t>
   </si>
@@ -239,9 +239,6 @@
     <t>carport</t>
   </si>
   <si>
-    <t>Ordner für die Datenablage</t>
-  </si>
-  <si>
     <t>SP_Sim</t>
   </si>
   <si>
@@ -509,15 +506,6 @@
     <t>Aus dem PV Input_File übernommen</t>
   </si>
   <si>
-    <t>Daten_Input\Beispiel_Lastgang_einlesen.xlsx</t>
-  </si>
-  <si>
-    <t>Daten_Input\Beispiel_LKW_Fahrdaten.xlsx</t>
-  </si>
-  <si>
-    <t>Daten_Input\Beispiel_PV_Input_aus_Polysun.xlsx</t>
-  </si>
-  <si>
     <t>A_Bedarf</t>
   </si>
   <si>
@@ -642,6 +630,24 @@
   </si>
   <si>
     <t>soc_fuer_wechsel</t>
+  </si>
+  <si>
+    <t>Ordner für die einzulesenden Daten</t>
+  </si>
+  <si>
+    <t>Daten_Input</t>
+  </si>
+  <si>
+    <t>r_DIR</t>
+  </si>
+  <si>
+    <t>Beispiel_Lastgang_einlesen.xlsx</t>
+  </si>
+  <si>
+    <t>Beispiel_PV_Input_aus_Polysun.xlsx</t>
+  </si>
+  <si>
+    <t>Beispiel_LKW_Fahrdaten.xlsx</t>
   </si>
 </sst>
 </file>
@@ -1195,7 +1201,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="62.4">
       <c r="A1" s="39" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="28.8">
@@ -1205,22 +1211,22 @@
     </row>
     <row r="3" spans="1:1" ht="28.8">
       <c r="A3" s="35" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="36" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="37" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="38" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -1278,7 +1284,7 @@
         <v>48</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C2" s="26" t="s">
         <v>7</v>
@@ -1289,10 +1295,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="6" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C3" s="26" t="s">
         <v>7</v>
@@ -1306,7 +1312,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C4" s="26" t="s">
         <v>7</v>
@@ -1317,10 +1323,10 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C5" s="26" t="s">
         <v>7</v>
@@ -1362,7 +1368,7 @@
         <v>38</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C8" s="26" t="s">
         <v>7</v>
@@ -1373,16 +1379,16 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C9" s="26" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1395,8 +1401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D42DFEB6-5036-45B9-BE08-6F41ED8602E3}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.109375" defaultRowHeight="14.4"/>
@@ -1427,10 +1433,10 @@
         <v>9</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>3</v>
@@ -1439,10 +1445,14 @@
     <row r="3" spans="1:4" s="12" customFormat="1">
       <c r="A3" s="10"/>
       <c r="B3" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="11"/>
+        <v>195</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>196</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="4" spans="1:4" s="12" customFormat="1" ht="28.8">
       <c r="A4" s="10" t="s">
@@ -1452,7 +1462,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>154</v>
+        <v>198</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>5</v>
@@ -1463,10 +1473,10 @@
         <v>11</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>156</v>
+        <v>199</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>13</v>
@@ -1480,7 +1490,7 @@
         <v>34</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>155</v>
+        <v>200</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>35</v>
@@ -1525,7 +1535,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="6" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B2" s="26">
         <v>1</v>
@@ -1534,7 +1544,7 @@
         <v>19</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1637,58 +1647,58 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B10" s="29">
         <v>0.25</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B11" s="29">
         <v>0.83333333333333337</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B12" s="29">
         <v>0.25</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B13" s="29">
         <v>0.54166666666666663</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1733,10 +1743,10 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="6" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C2" s="34" t="str">
         <f>Input!C5</f>
@@ -1754,7 +1764,7 @@
         <v>52</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C3" s="21">
         <v>0</v>
@@ -1763,7 +1773,7 @@
         <v>51</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="12" customFormat="1">
@@ -1856,7 +1866,7 @@
         <v>52</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C9" s="21">
         <v>300</v>
@@ -1870,10 +1880,10 @@
     </row>
     <row r="10" spans="1:5" s="12" customFormat="1" ht="43.2">
       <c r="A10" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C10" s="22" t="s">
         <v>7</v>
@@ -1882,32 +1892,32 @@
         <v>19</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="12" customFormat="1">
       <c r="A11" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C11" s="22">
         <v>0</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="12" customFormat="1">
       <c r="A12" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C12" s="25">
         <v>0.01</v>
@@ -1916,15 +1926,15 @@
         <v>19</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="12" customFormat="1">
       <c r="A13" s="10" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C13" s="25" t="s">
         <v>7</v>
@@ -1933,58 +1943,58 @@
         <v>19</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="12" customFormat="1" ht="28.8">
       <c r="A14" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C14" s="22">
         <v>0</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="12" customFormat="1">
       <c r="A15" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="B15" s="10" t="s">
         <v>152</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>153</v>
       </c>
       <c r="C15" s="22">
         <v>4.6399999999999997</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="12" customFormat="1">
       <c r="A16" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C16" s="22">
         <v>70</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -2030,10 +2040,10 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="6" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C2" s="34" t="str">
         <f>Input!C9</f>
@@ -2058,7 +2068,7 @@
         <v>19</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="12" customFormat="1">
@@ -2066,24 +2076,24 @@
         <v>41</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C4" s="22">
         <v>136</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="12" customFormat="1" ht="86.4">
       <c r="A5" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C5" s="21">
         <v>0</v>
@@ -2092,15 +2102,15 @@
         <v>19</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="12" customFormat="1">
       <c r="A6" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C6" s="23">
         <v>0.1</v>
@@ -2109,15 +2119,15 @@
         <v>19</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="12" customFormat="1">
       <c r="A7" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C7" s="23">
         <v>1</v>
@@ -2126,15 +2136,15 @@
         <v>19</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="12" customFormat="1">
       <c r="A8" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C8" s="24">
         <v>0.1</v>
@@ -2143,32 +2153,32 @@
         <v>19</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="12" customFormat="1">
       <c r="A9" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C9" s="21">
         <v>50</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="12" customFormat="1" ht="43.2">
       <c r="A10" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C10" s="22" t="s">
         <v>7</v>
@@ -2177,15 +2187,15 @@
         <v>19</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="12" customFormat="1">
       <c r="A11" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C11" s="22">
         <v>0</v>
@@ -2194,15 +2204,15 @@
         <v>25</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="12" customFormat="1">
       <c r="A12" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C12" s="25">
         <v>0.01</v>
@@ -2211,12 +2221,12 @@
         <v>19</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="12" customFormat="1">
       <c r="A13" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B13" s="10"/>
       <c r="C13" s="24">
@@ -2226,7 +2236,7 @@
         <v>19</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -2271,10 +2281,10 @@
     </row>
     <row r="2" spans="1:5" s="12" customFormat="1">
       <c r="A2" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>114</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>115</v>
       </c>
       <c r="C2" s="15">
         <f>Input!C6</f>
@@ -2289,24 +2299,24 @@
     </row>
     <row r="3" spans="1:5" s="12" customFormat="1">
       <c r="A3" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C3" s="17">
         <v>42</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="12" customFormat="1">
       <c r="A4" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B4" s="13"/>
       <c r="C4" s="16">
@@ -2316,64 +2326,64 @@
         <v>19</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="12" customFormat="1">
       <c r="A5" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C5" s="40">
         <v>0.63</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="12" customFormat="1" ht="28.8">
       <c r="A6" s="10" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C6" s="18">
         <v>90</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="12" customFormat="1">
       <c r="A7" s="10" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B7" s="13"/>
       <c r="C7" s="18">
         <v>100</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="12" customFormat="1">
       <c r="A8" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C8" s="19">
         <v>0</v>
@@ -2382,15 +2392,15 @@
         <v>19</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="12" customFormat="1">
       <c r="A9" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C9" s="19">
         <v>0.1</v>
@@ -2399,15 +2409,15 @@
         <v>19</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="12" customFormat="1" ht="28.8">
       <c r="A10" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C10" s="19">
         <v>0.05</v>
@@ -2416,7 +2426,7 @@
         <v>19</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -2428,7 +2438,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF14071F-F3CE-4A0E-9532-DB104DCFD8B6}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -2461,10 +2471,10 @@
     </row>
     <row r="2" spans="1:5" s="12" customFormat="1">
       <c r="A2" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>114</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>115</v>
       </c>
       <c r="C2" s="15">
         <f>Input!C7</f>
@@ -2479,24 +2489,24 @@
     </row>
     <row r="3" spans="1:5" s="12" customFormat="1">
       <c r="A3" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C3" s="17">
         <v>42</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="12" customFormat="1">
       <c r="A4" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B4" s="13"/>
       <c r="C4" s="16">
@@ -2506,49 +2516,49 @@
         <v>19</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="12" customFormat="1">
       <c r="A5" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C5" s="40">
         <v>0.63</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="12" customFormat="1" ht="28.8">
       <c r="A6" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C6" s="18">
         <v>90</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="12" customFormat="1" ht="28.8">
       <c r="A7" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C7" s="19">
         <v>0</v>
@@ -2557,15 +2567,15 @@
         <v>19</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="12" customFormat="1">
       <c r="A8" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C8" s="19">
         <v>0.1</v>
@@ -2574,15 +2584,15 @@
         <v>19</v>
       </c>
       <c r="E8" s="41" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="12" customFormat="1" ht="28.8">
       <c r="A9" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C9" s="19">
         <v>0.1</v>
@@ -2591,7 +2601,7 @@
         <v>19</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -2640,7 +2650,7 @@
         <v>38</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C2" s="30" t="str">
         <f>Input!C8</f>
@@ -2655,10 +2665,10 @@
     </row>
     <row r="3" spans="1:5" s="12" customFormat="1">
       <c r="A3" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="B3" s="13" t="s">
         <v>135</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>136</v>
       </c>
       <c r="C3" s="21">
         <v>10</v>
@@ -2667,64 +2677,64 @@
         <v>19</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="12" customFormat="1">
       <c r="A4" s="10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B4" s="13"/>
       <c r="C4" s="22">
         <v>68</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="12" customFormat="1" ht="28.8">
       <c r="A5" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="B5" s="13" t="s">
         <v>138</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>139</v>
       </c>
       <c r="C5" s="31">
         <v>10</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="12" customFormat="1">
       <c r="A6" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C6" s="32">
         <v>22</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="12" customFormat="1">
       <c r="A7" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="B7" s="13" t="s">
         <v>141</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>142</v>
       </c>
       <c r="C7" s="23">
         <v>0.25</v>
@@ -2733,15 +2743,15 @@
         <v>19</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="12" customFormat="1">
       <c r="A8" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="B8" s="13" t="s">
         <v>143</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>144</v>
       </c>
       <c r="C8" s="23">
         <v>0.5</v>
@@ -2750,7 +2760,7 @@
         <v>19</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>